<commit_message>
On the first page of the No Contact report, the choices should be: Yes, no follow-up needed; No, client needs care; and Unknown, client not reached. #9
</commit_message>
<xml_diff>
--- a/zazic-scale-up/forms/app/no_contact.xlsx
+++ b/zazic-scale-up/forms/app/no_contact.xlsx
@@ -1,14 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech-6\zazic-scale-up\forms\app\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C0FC87B-1824-43CE-BAC5-40B73F5D05E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="survey" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="choices" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="settings" sheetId="3" r:id="rId6"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataSignature="AMtx7mikWwwKiNNp4j7xL3IsWOSG8+uPXQ=="/>
@@ -53,22 +62,13 @@
     <t>yes</t>
   </si>
   <si>
-    <t>Yes, No follow up needed</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
     <t>instance_name</t>
   </si>
   <si>
-    <t>No, Client needs care</t>
-  </si>
-  <si>
     <t>unknown</t>
-  </si>
-  <si>
-    <t>Unknown</t>
   </si>
   <si>
     <t>formId</t>
@@ -254,85 +254,94 @@
   <si>
     <t>${additional_notes_text}</t>
   </si>
+  <si>
+    <t>No, client needs care</t>
+  </si>
+  <si>
+    <t>Unknown, client not reached</t>
+  </si>
+  <si>
+    <t>Yes, no follow-up needed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="14">
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Cambria"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Proxima Nova"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF843C0B"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF833C0C"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF843C0B"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF548135"/>
       <name val="Cambria"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
@@ -342,7 +351,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -352,7 +361,13 @@
     </fill>
   </fills>
   <borders count="3">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FFD0CECE"/>
@@ -366,122 +381,95 @@
       <bottom style="thin">
         <color rgb="FFD0CECE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="28">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="2" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -671,33 +659,33 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.33"/>
-    <col customWidth="1" min="2" max="2" width="19.11"/>
-    <col customWidth="1" min="3" max="3" width="44.44"/>
-    <col customWidth="1" min="4" max="4" width="37.22"/>
-    <col customWidth="1" min="5" max="5" width="9.33"/>
-    <col customWidth="1" min="6" max="7" width="11.44"/>
-    <col customWidth="1" min="8" max="8" width="34.0"/>
-    <col customWidth="1" min="9" max="26" width="11.44"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="3" max="3" width="44.5" customWidth="1"/>
+    <col min="4" max="4" width="37.25" customWidth="1"/>
+    <col min="5" max="5" width="9.375" customWidth="1"/>
+    <col min="6" max="7" width="11.5" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
+    <col min="9" max="26" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" ht="15.75">
       <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
@@ -708,28 +696,28 @@
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="K1" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
@@ -747,128 +735,128 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" ht="15.75">
       <c r="A2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="E2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="14" t="s">
+    </row>
+    <row r="3" spans="1:26" ht="15.75">
+      <c r="A3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C3" s="14" t="s">
         <v>37</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3">
-      <c r="A3" s="13" t="s">
+    <row r="4" spans="1:26" ht="15.75">
+      <c r="A4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="1" t="s">
+    </row>
+    <row r="5" spans="1:26" ht="15.75">
+      <c r="A5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>42</v>
       </c>
+      <c r="C5" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="4">
-      <c r="A4" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="16" t="s">
+    <row r="6" spans="1:26" ht="15.75">
+      <c r="A6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>41</v>
+      <c r="B6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7">
+    <row r="7" spans="1:26" ht="15.75">
       <c r="A7" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:26" ht="15.75">
       <c r="A8" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:26" ht="15.75">
       <c r="A9" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="17"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:26" ht="15.75">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="17"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:26" ht="15.75">
       <c r="A11" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20"/>
@@ -878,7 +866,7 @@
       <c r="I11" s="20"/>
       <c r="J11" s="20"/>
       <c r="K11" s="20" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
@@ -896,15 +884,15 @@
       <c r="Y11" s="20"/>
       <c r="Z11" s="20"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:26" ht="15.75">
       <c r="A12" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="22" t="s">
-        <v>59</v>
-      </c>
       <c r="C12" s="22" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="22" t="s">
@@ -914,7 +902,7 @@
       <c r="H12" s="18"/>
       <c r="J12" s="20"/>
       <c r="K12" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L12" s="20"/>
       <c r="M12" s="20"/>
@@ -932,15 +920,15 @@
       <c r="Y12" s="20"/>
       <c r="Z12" s="20"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:26" ht="15.75">
       <c r="A13" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -950,7 +938,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
@@ -968,19 +956,19 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:26" ht="15.75">
       <c r="A14" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D14" s="25"/>
       <c r="E14" s="25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F14" s="25"/>
       <c r="G14" s="25"/>
@@ -1004,15 +992,15 @@
       <c r="Y14" s="25"/>
       <c r="Z14" s="25"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:26" ht="143.25">
       <c r="A15" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
@@ -1038,15 +1026,15 @@
       <c r="Y15" s="25"/>
       <c r="Z15" s="25"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:26" ht="15.75">
       <c r="A16" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D16" s="25"/>
       <c r="E16" s="25"/>
@@ -1074,27 +1062,27 @@
       <c r="Y16" s="25"/>
       <c r="Z16" s="25"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:26" ht="15.75">
       <c r="A17" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G17" s="25"/>
       <c r="H17" s="25"/>
       <c r="I17" s="25"/>
       <c r="J17" s="25"/>
       <c r="K17" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="L17" s="25"/>
       <c r="M17" s="25"/>
@@ -1112,20 +1100,20 @@
       <c r="Y17" s="25"/>
       <c r="Z17" s="25"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:26" ht="15.75">
       <c r="A18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C18" s="27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="25"/>
       <c r="F18" s="25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
@@ -1148,9 +1136,9 @@
       <c r="Y18" s="25"/>
       <c r="Z18" s="25"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:26" ht="15.75" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="23"/>
@@ -1178,19 +1166,19 @@
       <c r="Y19" s="25"/>
       <c r="Z19" s="25"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1"/>
-    <row r="21" ht="15.75" customHeight="1"/>
-    <row r="22" ht="15.75" customHeight="1"/>
-    <row r="23" ht="15.75" customHeight="1"/>
-    <row r="24" ht="15.75" customHeight="1"/>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="21" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="22" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="25" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="26" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="27" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="28" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="29" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="30" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="31" spans="1:26" ht="15.75" customHeight="1"/>
+    <row r="32" spans="1:26" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1"/>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -2155,34 +2143,30 @@
     <row r="994" ht="15.75" customHeight="1"/>
     <row r="995" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:C972"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.44"/>
-    <col customWidth="1" min="2" max="2" width="11.44"/>
-    <col customWidth="1" min="3" max="3" width="17.78"/>
-    <col customWidth="1" min="4" max="6" width="11.44"/>
-    <col customWidth="1" min="7" max="26" width="8.56"/>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="4" max="6" width="11.5" customWidth="1"/>
+    <col min="7" max="26" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2193,12 +2177,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2206,62 +2190,62 @@
         <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="11" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="12" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="14" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="15" spans="1:3" ht="15.75" customHeight="1"/>
+    <row r="16" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3219,32 +3203,28 @@
     <row r="971" ht="15.75" customHeight="1"/>
     <row r="972" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="31.89"/>
-    <col customWidth="1" min="2" max="2" width="43.67"/>
-    <col customWidth="1" min="3" max="3" width="32.89"/>
-    <col customWidth="1" min="4" max="4" width="20.89"/>
-    <col customWidth="1" min="5" max="15" width="11.44"/>
-    <col customWidth="1" min="16" max="26" width="8.78"/>
+    <col min="1" max="1" width="31.875" customWidth="1"/>
+    <col min="2" max="2" width="43.625" customWidth="1"/>
+    <col min="3" max="3" width="32.875" customWidth="1"/>
+    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="5" max="15" width="11.5" customWidth="1"/>
+    <col min="16" max="26" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
+    <row r="1" spans="1:26" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -3261,16 +3241,16 @@
         <v>9</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -3290,31 +3270,31 @@
       <c r="Y1" s="6"/>
       <c r="Z1" s="6"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="11">
-        <v>43896.0</v>
+        <v>43896</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J2" s="12"/>
       <c r="K2" s="12"/>
@@ -4315,9 +4295,7 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.984027777777778" footer="0.0" header="0.0" left="0.747916666666667" right="0.747916666666667" top="0.984027777777778"/>
+  <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>